<commit_message>
BugFix: Valve Timing config fixed for 05C331, 332, and 335
</commit_message>
<xml_diff>
--- a/ApplicationModules/ValveTiming/ValveTimingConfig_Pad_C.xlsx
+++ b/ApplicationModules/ValveTiming/ValveTimingConfig_Pad_C.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Documents/MATLAB/MDRT/ApplicationModules/ValveTiming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF837EF-B100-F441-94D8-959D6F5B811C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215106F3-D59E-2C45-8AA5-329F856904F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="800" windowWidth="38000" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38600" yWindow="800" windowWidth="38000" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -650,6 +650,72 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -961,72 +1027,6 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1107,29 +1107,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{611E65C7-1F07-D24B-ABB2-BBC2D61288CE}" name="Table3" displayName="Table3" ref="A1:J44" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{611E65C7-1F07-D24B-ABB2-BBC2D61288CE}" name="Table3" displayName="Table3" ref="A1:J44" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
   <autoFilter ref="A1:J44" xr:uid="{611E65C7-1F07-D24B-ABB2-BBC2D61288CE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F44">
     <sortCondition ref="B1:B44"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{638ECC2F-FC00-394B-AB29-829073FD95BD}" name="Valve Type" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{95B72D95-7126-2D4B-BD42-560378E2478B}" name="Valve FN" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{1C28C0B7-EB01-164F-BC1F-4AD0236C4ED4}" name="Open I/O" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{9063E8B3-5F15-DC4C-BA30-92C9AAD4F6D6}" name="Closed I/O" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{BB29291E-0D89-F244-AE14-AC9A7E43955A}" name="Command I/O" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{B03A0761-0C9D-7A43-BD9C-032D64245A32}" name="TRUE State Signal" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{B3C7DE10-4CF0-744E-AF56-5872B0CBD1CE}" name="Open_Min" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{F2C2894C-0FFC-CE44-945B-5AC19D5B6D2C}" name="Open_Max" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{B8195841-CBAB-374C-AD63-0BF72BDF04FF}" name="Close_Min" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{5556F2CA-6641-E448-831A-C2CE333008F3}" name="Close_Max" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{638ECC2F-FC00-394B-AB29-829073FD95BD}" name="Valve Type" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{95B72D95-7126-2D4B-BD42-560378E2478B}" name="Valve FN" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{1C28C0B7-EB01-164F-BC1F-4AD0236C4ED4}" name="Open I/O" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{9063E8B3-5F15-DC4C-BA30-92C9AAD4F6D6}" name="Closed I/O" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{BB29291E-0D89-F244-AE14-AC9A7E43955A}" name="Command I/O" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{B03A0761-0C9D-7A43-BD9C-032D64245A32}" name="TRUE State Signal" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{B3C7DE10-4CF0-744E-AF56-5872B0CBD1CE}" name="Open_Min" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{F2C2894C-0FFC-CE44-945B-5AC19D5B6D2C}" name="Open_Max" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{B8195841-CBAB-374C-AD63-0BF72BDF04FF}" name="Close_Min" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{5556F2CA-6641-E448-831A-C2CE333008F3}" name="Close_Max" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{298D4EDF-DA51-EC44-9717-E0E35FFCB297}" name="Table1" displayName="Table1" ref="A1:F46" totalsRowShown="0" headerRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{298D4EDF-DA51-EC44-9717-E0E35FFCB297}" name="Table1" displayName="Table1" ref="A1:F46" totalsRowShown="0" headerRowDxfId="10">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F46">
     <sortCondition ref="A1:A46"/>
   </sortState>
@@ -1138,10 +1138,10 @@
     <tableColumn id="2" xr3:uid="{429BA4B4-A157-A04B-AF7F-0E5FA003F2D8}" name="Component"/>
     <tableColumn id="3" xr3:uid="{17D0EC8C-E9F3-A444-8699-7A4FED5184E0}" name="Desc"/>
     <tableColumn id="4" xr3:uid="{B130B13B-B755-DE4B-B4C0-29A36437D8F2}" name="Connection"/>
-    <tableColumn id="5" xr3:uid="{774A9C8A-3E23-2641-94DE-21B4AEE9E95E}" name="Valve_Size" dataDxfId="22">
+    <tableColumn id="5" xr3:uid="{774A9C8A-3E23-2641-94DE-21B4AEE9E95E}" name="Valve_Size" dataDxfId="9">
       <calculatedColumnFormula array="1">size_from_connection(Table1[[#This Row],[Connection]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{270789F0-E690-4E43-9BF4-2487B6F0FA19}" name="Column1" dataDxfId="21">
+    <tableColumn id="6" xr3:uid="{270789F0-E690-4E43-9BF4-2487B6F0FA19}" name="Column1" dataDxfId="8">
       <calculatedColumnFormula>ISERROR(MATCH(Table1[[#This Row],[Find]],Table3[Valve FN],0))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1150,7 +1150,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2250AD48-524E-5C41-BCB3-74EB75269E3C}" name="Table2" displayName="Table2" ref="H1:I14" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2250AD48-524E-5C41-BCB3-74EB75269E3C}" name="Table2" displayName="Table2" ref="H1:I14" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="H1:I14" xr:uid="{2250AD48-524E-5C41-BCB3-74EB75269E3C}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{DD69C03E-E9C0-B841-889E-763E9D6FDE90}" name="BOM Connection"/>
@@ -1161,14 +1161,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A2F36033-04E7-8948-8621-5FB2281A5E32}" name="Table4" displayName="Table4" ref="L1:P10" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A2F36033-04E7-8948-8621-5FB2281A5E32}" name="Table4" displayName="Table4" ref="L1:P10" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="L1:P10" xr:uid="{A2F36033-04E7-8948-8621-5FB2281A5E32}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{F07B81A4-5B58-024C-9E32-3D0CF4EB9132}" name="Size"/>
-    <tableColumn id="2" xr3:uid="{8F007D28-9431-8549-BCC3-830A60D10A0E}" name="Open_Min" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{A259F2DD-38A9-F742-B639-ED2F509BACAF}" name="Open_Max" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{D44346DB-C3C9-3E4B-B6E1-84C1BDEB4876}" name="Close_Min" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{80242C8E-9B00-7B43-8D86-B90E45BBE06F}" name="Close_Max" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{8F007D28-9431-8549-BCC3-830A60D10A0E}" name="Open_Min" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{A259F2DD-38A9-F742-B639-ED2F509BACAF}" name="Open_Max" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{D44346DB-C3C9-3E4B-B6E1-84C1BDEB4876}" name="Close_Min" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{80242C8E-9B00-7B43-8D86-B90E45BBE06F}" name="Close_Max" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1440,8 +1440,8 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2469,8 +2469,8 @@
       <c r="E32" s="5">
         <v>599</v>
       </c>
-      <c r="F32" s="5">
-        <v>0</v>
+      <c r="F32" s="3">
+        <v>1</v>
       </c>
       <c r="G32" s="13">
         <v>0</v>
@@ -2501,8 +2501,8 @@
       <c r="E33" s="4">
         <v>606</v>
       </c>
-      <c r="F33" s="4">
-        <v>0</v>
+      <c r="F33" s="3">
+        <v>1</v>
       </c>
       <c r="G33" s="13">
         <v>0</v>
@@ -2533,8 +2533,8 @@
       <c r="E34" s="5">
         <v>603</v>
       </c>
-      <c r="F34" s="5">
-        <v>0</v>
+      <c r="F34" s="3">
+        <v>1</v>
       </c>
       <c r="G34" s="13">
         <v>0</v>

</xml_diff>